<commit_message>
create example + folder structure input and ouput
</commit_message>
<xml_diff>
--- a/00_input/hanzi_list.xlsx
+++ b/00_input/hanzi_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasvoss/Documents/Master Wirtschaftsphysik/3. Semester/anki_vocabulary_automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasvoss/Documents/anki_vocabulary_automation/00_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13D259B-F71D-AC4C-8AA9-C462076DFCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BCE98D-F5D7-C04C-86ED-0EACC906FFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{8949169C-D32D-FF47-B3A2-C1A222E5BCFD}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Hanzi</t>
+  </si>
+  <si>
+    <t>好</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,9 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:1" ht="20" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>

</xml_diff>